<commit_message>
parameter changes in output config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2735D71-5A10-4340-B8FC-17B6015115E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733628EC-405A-4B8C-B83D-60D90CD33312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Parameter</t>
   </si>
@@ -103,6 +103,39 @@
   </si>
   <si>
     <t>Print Plots?</t>
+  </si>
+  <si>
+    <t>Plot Parameter Changes</t>
+  </si>
+  <si>
+    <t>Plot Power</t>
+  </si>
+  <si>
+    <t>Plot Time</t>
+  </si>
+  <si>
+    <t>Plot Speed</t>
+  </si>
+  <si>
+    <t>Change Parameters</t>
+  </si>
+  <si>
+    <t>Change Power</t>
+  </si>
+  <si>
+    <t>Change Speed</t>
+  </si>
+  <si>
+    <t>Time for each layer</t>
+  </si>
+  <si>
+    <t>Power set for each layer</t>
+  </si>
+  <si>
+    <t>Speed set for each layer</t>
+  </si>
+  <si>
+    <t>This controls everything in green also. This row has to be set to Yes for Plot Power, Plot Speed, etc. to work</t>
   </si>
 </sst>
 </file>
@@ -134,12 +167,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,11 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,20 +513,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,12 +540,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -519,88 +559,177 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed and organized xml output
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23757779-FB19-4B10-A999-9E1AE131081D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D240A1-549F-4E5E-AD2A-95ACC6B924D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="18096" windowHeight="11580" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Output</t>
   </si>
   <si>
-    <t>nist.stl</t>
-  </si>
-  <si>
     <t xml:space="preserve">Part must be in the "geometry" folder. Include only the name of the file, not the full path. </t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Sort strategy for hatches</t>
+  </si>
+  <si>
+    <t>nut.stl</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -619,46 +619,46 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -668,144 +668,144 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -815,49 +815,49 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>0.08</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>0.06</v>
       </c>
       <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
         <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -873,16 +873,16 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert Excel file merge issue
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD50611-26CD-41E4-9C11-1611EA43B726}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D240A1-549F-4E5E-AD2A-95ACC6B924D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Parameter</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Output</t>
   </si>
   <si>
+    <t xml:space="preserve">Part must be in the "geometry" folder. Include only the name of the file, not the full path. </t>
+  </si>
+  <si>
     <t>Output .png?</t>
   </si>
   <si>
@@ -99,13 +102,94 @@
     <t>Print Plots?</t>
   </si>
   <si>
+    <t>Plot Parameter Changes</t>
+  </si>
+  <si>
+    <t>Plot Power</t>
+  </si>
+  <si>
+    <t>Plot Time</t>
+  </si>
+  <si>
+    <t>Plot Speed</t>
+  </si>
+  <si>
+    <t>Change Parameters</t>
+  </si>
+  <si>
+    <t>Change Power</t>
+  </si>
+  <si>
+    <t>Change Speed</t>
+  </si>
+  <si>
+    <t>Time for each layer</t>
+  </si>
+  <si>
+    <t>Power set for each layer</t>
+  </si>
+  <si>
+    <t>Speed set for each layer</t>
+  </si>
+  <si>
+    <t>This controls everything in green also. This row has to be set to Yes for Plot Power, Plot Speed, etc. to work</t>
+  </si>
+  <si>
+    <t>Plot Jump Vectors</t>
+  </si>
+  <si>
+    <t>Scan Strategy</t>
+  </si>
+  <si>
+    <t>Island</t>
+  </si>
+  <si>
+    <t>Hatch Angle</t>
+  </si>
+  <si>
+    <t>Volume of Offset Hatch</t>
+  </si>
+  <si>
+    <t>An angle in degrees 0-90, e.g. 45</t>
+  </si>
+  <si>
+    <t>[mm] e.g. .08</t>
+  </si>
+  <si>
+    <t>Spot Compensation</t>
+  </si>
+  <si>
+    <t>Hatch angle for the islands</t>
+  </si>
+  <si>
+    <t>Offset between internal and external boundary</t>
+  </si>
+  <si>
+    <t>[mm] e.g. .06</t>
+  </si>
+  <si>
+    <t>Additional offset to account for laser spot size</t>
+  </si>
+  <si>
+    <t>Number of Inner Contours</t>
+  </si>
+  <si>
+    <t>Number of Outer Contours</t>
+  </si>
+  <si>
+    <t>Hatching Sort Method</t>
+  </si>
+  <si>
+    <t>Alternate</t>
+  </si>
+  <si>
+    <t>Alternate/Linear/Greedy</t>
+  </si>
+  <si>
+    <t>Sort strategy for hatches</t>
+  </si>
+  <si>
     <t>nut.stl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Part must be in the "geometry" folder. Include only the name and extension of the file (i.e. nut.stl), not the full path. </t>
-  </si>
-  <si>
-    <t>Plot Jumps</t>
   </si>
 </sst>
 </file>
@@ -137,12 +221,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,11 +253,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,20 +574,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,125 +595,294 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>0.08</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>0.06</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More misc. merge conflict changes (probably broke some stuff, sorry!)
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D240A1-549F-4E5E-AD2A-95ACC6B924D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C72AD2-AF5D-4E82-A62B-7CEFBF3E76FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,17 +577,17 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.109375" customWidth="1"/>
+    <col min="1" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,12 +601,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -614,7 +614,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -628,29 +628,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -661,12 +661,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -680,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -694,7 +694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -708,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -719,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -730,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -741,7 +741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -752,7 +752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -766,7 +766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -780,7 +780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -794,7 +794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
@@ -808,12 +808,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
@@ -827,7 +827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
@@ -841,7 +841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -855,7 +855,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -871,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Debug output for input options
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23360632-4D2B-4488-8427-569D9D23566B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A9EDE-1EF2-4FFF-B79C-1802E817238A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
     <t>Parameter</t>
   </si>
@@ -180,16 +180,25 @@
     <t>Hatching Sort Method</t>
   </si>
   <si>
-    <t>Alternate</t>
-  </si>
-  <si>
-    <t>Alternate/Linear/Greedy</t>
-  </si>
-  <si>
     <t>Sort strategy for hatches</t>
   </si>
   <si>
     <t>nut.stl</t>
+  </si>
+  <si>
+    <t>None/Alternate/Linear/Greedy</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Write Debug?</t>
+  </si>
+  <si>
+    <t>Outputs to a file named debug.txt</t>
   </si>
 </sst>
 </file>
@@ -253,13 +262,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,21 +584,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="92" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -600,13 +612,25 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -614,12 +638,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -628,8 +652,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
@@ -639,8 +663,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
@@ -650,8 +674,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
@@ -661,13 +685,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
@@ -680,8 +704,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
@@ -694,12 +718,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -708,8 +732,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
@@ -719,8 +743,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
@@ -730,8 +754,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
@@ -741,8 +765,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
@@ -753,11 +777,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -767,7 +791,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -781,7 +805,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -795,7 +819,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -814,7 +838,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B24">
@@ -828,7 +852,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B25">
@@ -842,7 +866,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B26">
@@ -856,7 +880,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B27">
@@ -864,7 +888,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B28">
@@ -872,17 +896,36 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>50</v>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change config to realistic run params
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A9EDE-1EF2-4FFF-B79C-1802E817238A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA038478-0428-49CA-B672-BF82CBE4F4AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Parameter</t>
   </si>
@@ -87,9 +87,6 @@
     <t>File Name</t>
   </si>
   <si>
-    <t>If set to no, no images, etc. will be output regardless of their values.</t>
-  </si>
-  <si>
     <t>Plot Contours</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Plot Centroids</t>
   </si>
   <si>
-    <t>Print Plots?</t>
-  </si>
-  <si>
     <t>Plot Parameter Changes</t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>Outputs to a file named debug.txt</t>
+  </si>
+  <si>
+    <t>Output Plots?</t>
+  </si>
+  <si>
+    <t>If set to no, nothing in this section matters.</t>
   </si>
 </sst>
 </file>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +599,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,38 +612,26 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -652,9 +640,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -663,9 +651,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -674,9 +662,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -685,14 +673,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -701,10 +689,10 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,7 +706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -732,31 +720,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -765,9 +753,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -778,7 +766,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -787,12 +775,12 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
@@ -801,12 +789,12 @@
         <v>10</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
@@ -815,12 +803,12 @@
         <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>13</v>
@@ -829,7 +817,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,49 +827,49 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>0.08</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>0.06</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -889,7 +877,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -897,26 +885,26 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -925,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read areas and scanpaths from excel
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA038478-0428-49CA-B672-BF82CBE4F4AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B2F63-DCC8-4221-A3AC-C064CAAF71D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scan Path Switching" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Parameter</t>
   </si>
@@ -199,6 +200,42 @@
   </si>
   <si>
     <t>If set to no, nothing in this section matters.</t>
+  </si>
+  <si>
+    <t>min_x</t>
+  </si>
+  <si>
+    <t>min_y</t>
+  </si>
+  <si>
+    <t>min_z</t>
+  </si>
+  <si>
+    <t>max_x</t>
+  </si>
+  <si>
+    <t>max_y</t>
+  </si>
+  <si>
+    <t>max_z</t>
+  </si>
+  <si>
+    <t>Note: Capitalization Matters</t>
+  </si>
+  <si>
+    <t>Note: Any unspecified areas will have `default` hatching applied to them</t>
+  </si>
+  <si>
+    <t>scanpath</t>
+  </si>
+  <si>
+    <t>Eligible `scanpath` Values: `default`, `island`</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>frick</t>
   </si>
 </sst>
 </file>
@@ -586,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,4 +957,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E748D16C-34BB-49DF-BFFD-DBF0524D3346}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish Excel file input (except id linking)
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B2F63-DCC8-4221-A3AC-C064CAAF71D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD98A541-3B39-4B55-A708-732B3F98E55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Scan Path Switching" sheetId="2" r:id="rId2"/>
+    <sheet name="1. General" sheetId="1" r:id="rId1"/>
+    <sheet name="2. SPS - Area Specification" sheetId="2" r:id="rId2"/>
+    <sheet name="3. SPS - Generic Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="4. SPS - Custom Parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
   <si>
     <t>Parameter</t>
   </si>
@@ -220,29 +222,272 @@
     <t>max_z</t>
   </si>
   <si>
-    <t>Note: Capitalization Matters</t>
-  </si>
-  <si>
-    <t>Note: Any unspecified areas will have `default` hatching applied to them</t>
-  </si>
-  <si>
     <t>scanpath</t>
   </si>
   <si>
-    <t>Eligible `scanpath` Values: `default`, `island`</t>
-  </si>
-  <si>
     <t>island</t>
   </si>
   <si>
-    <t>frick</t>
+    <t>Param 1</t>
+  </si>
+  <si>
+    <t>Param 2</t>
+  </si>
+  <si>
+    <t>Param 3</t>
+  </si>
+  <si>
+    <t>Param 5</t>
+  </si>
+  <si>
+    <t>Param 4</t>
+  </si>
+  <si>
+    <t># Inner Contours</t>
+  </si>
+  <si>
+    <t># Outer Contours</t>
+  </si>
+  <si>
+    <t>Hatch Distance (mm)</t>
+  </si>
+  <si>
+    <t>Hatch Angle (mm)</t>
+  </si>
+  <si>
+    <t>Layer Angle Increment (deg)</t>
+  </si>
+  <si>
+    <t>Hatch Sort Method</t>
+  </si>
+  <si>
+    <t>Area ID</t>
+  </si>
+  <si>
+    <t>Spot Compensation (Multiple)</t>
+  </si>
+  <si>
+    <t>Volume Offset Hatch (mm)</t>
+  </si>
+  <si>
+    <t>Explanations:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch Distance: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance between hatches.</t>
+    </r>
+  </si>
+  <si>
+    <t>Unit: Degrees</t>
+  </si>
+  <si>
+    <t>Unit: mm</t>
+  </si>
+  <si>
+    <t>Recommended/Default: &lt;TODO&gt;</t>
+  </si>
+  <si>
+    <t>Recommended/Default: 66.7</t>
+  </si>
+  <si>
+    <t>Recommended/Default: 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch Angle: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The initial hatch angle on layer zero. Unit circle conventions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Layer Angle Increment: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Degree change per layer. Unit circle conventions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Valid Values: `None`, `Alternate`, `Linear`, `Greedy`</t>
+  </si>
+  <si>
+    <t>None: Do not apply any reordering.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch Sort Method: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The ordering / "sorting" method applied to the hatches.</t>
+    </r>
+  </si>
+  <si>
+    <t>Alternate: &lt;TODO: Figure out what this is&gt;</t>
+  </si>
+  <si>
+    <t>Linear: &lt;TODO: Figure out what this is&gt;</t>
+  </si>
+  <si>
+    <t>Greedy: &lt;TODO: Figure out what this is&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Inner Contours: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number of inner contours; pretty self-explanatory.</t>
+    </r>
+  </si>
+  <si>
+    <t>Unit: Unitless</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Outer Contours: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number of outer contours; pretty self-explanatory.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spot Compensation: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A factor controlling the distance to offset the outer contours and inner hatching.</t>
+    </r>
+  </si>
+  <si>
+    <t>Recommended/Default: 1</t>
+  </si>
+  <si>
+    <t>Recommended/Default: 1 (i.e. no change)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume Offset Hatch: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Additional distance offset between contours and hatches.</t>
+    </r>
+  </si>
+  <si>
+    <t>Recommended/Default: 0 (i.e. no offset)</t>
+  </si>
+  <si>
+    <t>This sheet is where you can specify any custom parameters for each scan path. The ordering for each scan path is given below:</t>
+  </si>
+  <si>
+    <t>Island:</t>
+  </si>
+  <si>
+    <t>Param 1: Island Size (mm); Recommended 5mm.</t>
+  </si>
+  <si>
+    <t>Default:</t>
+  </si>
+  <si>
+    <t>No parameters. Any value entered will be ignored.</t>
+  </si>
+  <si>
+    <t>Param 2: Island Overlap (mm); Recommended .1mm</t>
+  </si>
+  <si>
+    <t>Param 3: Island Offset (mm); Recommended 1mm</t>
+  </si>
+  <si>
+    <t>On this sheet, specify any parameters common to all the hatching methods.</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Eligible Scanpaths (capitalization matters):</t>
+  </si>
+  <si>
+    <t>To use this sheet:</t>
+  </si>
+  <si>
+    <t>1. Fill in the bounding box for the area, as well as the scanpath type you want to apply it (valid types found below).</t>
+  </si>
+  <si>
+    <t>2. For the given ID, on Sheet 3, fill out all the generic parameters that you want to be applied to that one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. For the given ID, on Sheet 4, fill out any scanpath-specific parameters. Not necessary for `default`. </t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>NOTE: ids don't actually link correctly yet; just make sure each area is in the same order on each sheet (i.e. in the same "row" across sheets).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +506,21 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -299,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,6 +567,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,117 +1223,588 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E748D16C-34BB-49DF-BFFD-DBF0524D3346}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9024CE-A5DF-42F3-AE7B-2A4DCBB48BEC}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>6</v>
+      </c>
+      <c r="H3" s="7">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7">
+        <v>6</v>
+      </c>
+      <c r="H4" s="7">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7">
+        <v>8</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K16" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K18" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K19" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K20" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K21" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K23" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K24" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K25" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K27" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K28" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K29" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K31" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K32" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K33" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K35" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K36" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K37" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DF6AF3-E694-4A6C-AA71-04288AE4F8F9}">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="7">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="7">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="7">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="7">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="H2" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C3" s="7">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="7">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="7">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="7">
         <v>6</v>
       </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="8"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="8"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H25" s="8"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="8"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
xml debug, hdf5 output, misc
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA038478-0428-49CA-B672-BF82CBE4F4AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4244EB-2913-48A9-86C3-882AFE223059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,35 +177,35 @@
     <t>Sort strategy for hatches</t>
   </si>
   <si>
+    <t>None/Alternate/Linear/Greedy</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Write Debug?</t>
+  </si>
+  <si>
+    <t>Outputs to a file named debug.txt</t>
+  </si>
+  <si>
+    <t>Output Plots?</t>
+  </si>
+  <si>
+    <t>If set to no, nothing in this section matters.</t>
+  </si>
+  <si>
     <t>nut.stl</t>
-  </si>
-  <si>
-    <t>None/Alternate/Linear/Greedy</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>Write Debug?</t>
-  </si>
-  <si>
-    <t>Outputs to a file named debug.txt</t>
-  </si>
-  <si>
-    <t>Output Plots?</t>
-  </si>
-  <si>
-    <t>If set to no, nothing in this section matters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +225,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -587,19 +593,19 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="92" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,12 +619,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -626,12 +632,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -640,29 +646,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -673,31 +679,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -706,12 +712,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -720,7 +726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -731,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -742,7 +748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -753,7 +759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -764,12 +770,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -778,12 +784,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>10</v>
@@ -792,12 +798,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
@@ -806,7 +812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -820,12 +826,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -839,7 +845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -853,7 +859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -867,7 +873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -875,7 +881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -883,40 +889,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
         <v>51</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
jump vectors in XML, workflow improvements
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\CDME\ScanningPrintingPaths\cdme-scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4244EB-2913-48A9-86C3-882AFE223059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6A10F4-31EC-4B8A-9DFC-E98C0E569C2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Parameter</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>nut.stl</t>
+  </si>
+  <si>
+    <t>Trajectory Ordering</t>
+  </si>
+  <si>
+    <t>Contour First?</t>
   </si>
 </sst>
 </file>
@@ -590,9 +596,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -922,6 +928,19 @@
         <v>51</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement default hatcher modifiability
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\cdme-scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD98A541-3B39-4B55-A708-732B3F98E55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC80FCE4-4E9A-4655-A86C-702CC0AAA5E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="1. General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
   <si>
     <t>Parameter</t>
   </si>
@@ -468,6 +468,18 @@
     <t>To use this sheet:</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>NOTE: ids don't actually link correctly yet; just make sure each area is in the same order on each sheet (i.e. in the same "row" across sheets).</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>1. Fill in the bounding box for the area, as well as the scanpath type you want to apply it (valid types found below).</t>
   </si>
   <si>
@@ -477,10 +489,10 @@
     <t xml:space="preserve">3. For the given ID, on Sheet 4, fill out any scanpath-specific parameters. Not necessary for `default`. </t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>NOTE: ids don't actually link correctly yet; just make sure each area is in the same order on each sheet (i.e. in the same "row" across sheets).</t>
+    <t>Note that area specification for the default does nothing; the scan path matters, though.</t>
+  </si>
+  <si>
+    <t>&lt;-- Default Scan Path</t>
   </si>
 </sst>
 </file>
@@ -889,16 +901,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="92" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -912,12 +924,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -925,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -939,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -950,7 +962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -961,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -972,12 +984,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1091,7 +1103,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1119,12 +1131,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -1166,7 +1178,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -1174,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -1182,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1196,12 +1208,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -1226,18 +1238,20 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>55</v>
@@ -1260,125 +1274,164 @@
       <c r="H1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
       </c>
       <c r="H3" t="s">
         <v>62</v>
       </c>
-      <c r="J3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
       </c>
       <c r="H4" t="s">
         <v>62</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J8" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J10" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="17:17" x14ac:dyDescent="0.3">
       <c r="Q17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1387,24 +1440,24 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="19.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="19.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1436,9 +1489,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>0</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
@@ -1468,9 +1521,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -1497,9 +1550,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
@@ -1529,132 +1582,159 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7">
+        <v>6</v>
+      </c>
+      <c r="H5" s="7">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7">
+        <v>8</v>
+      </c>
       <c r="K5" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K6" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K8" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K9" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K10" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K12" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K21" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K23" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K24" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K25" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K27" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K28" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K29" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K31" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K32" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K33" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K35" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K36" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K37" s="7" t="s">
         <v>99</v>
       </c>
@@ -1669,15 +1749,15 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>74</v>
       </c>
@@ -1700,32 +1780,32 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
       <c r="C2" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7">
         <v>6</v>
@@ -1743,9 +1823,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
@@ -1766,44 +1846,62 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
       <c r="H5" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H7" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H8" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H9" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H10" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H14" s="8"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H21" s="8"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H25" s="8"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H29" s="8"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H33" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc fixes; still fixing integer truncation import issue
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\cdme-scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC80FCE4-4E9A-4655-A86C-702CC0AAA5E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BCD9D8-C324-4CF2-8C67-41B2D581D001}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
   <sheets>
     <sheet name="1. General" sheetId="1" r:id="rId1"/>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7AC80-D3E1-4CD6-AC47-9D4F4439929B}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E748D16C-34BB-49DF-BFFD-DBF0524D3346}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1439,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9024CE-A5DF-42F3-AE7B-2A4DCBB48BEC}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1494,28 +1494,28 @@
         <v>113</v>
       </c>
       <c r="B2" s="7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>3</v>
+        <v>66.7</v>
       </c>
       <c r="E2" s="7">
         <v>4</v>
       </c>
       <c r="F2" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H2" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I2" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>107</v>
@@ -1526,28 +1526,28 @@
         <v>0</v>
       </c>
       <c r="B3" s="7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="7">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7">
-        <v>3</v>
+        <v>66.7</v>
       </c>
       <c r="E3" s="7">
         <v>4</v>
       </c>
       <c r="F3" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H3" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1555,28 +1555,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="7">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="D4" s="7">
-        <v>3</v>
+        <v>66.7</v>
       </c>
       <c r="E4" s="7">
         <v>4</v>
       </c>
       <c r="F4" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H4" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>78</v>
@@ -1587,28 +1587,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="7">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="D5" s="7">
-        <v>3</v>
+        <v>66.7</v>
       </c>
       <c r="E5" s="7">
         <v>4</v>
       </c>
       <c r="F5" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H5" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Imperfect, but very close
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aacit\OneDrive\Documents\scangen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE481FD-1BCA-41C4-B481-AFB24594B483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FAC1B7-8AD5-4C46-815B-9BA1B4716825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4C8709F-E8C8-45E4-A788-6BA79573D54A}"/>
   </bookViews>
@@ -911,7 +911,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1082,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,22 +1322,22 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>-100</v>
+        <v>-32</v>
       </c>
       <c r="C3">
         <v>-100</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>-28</v>
       </c>
       <c r="F3">
         <v>100</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>62</v>

</xml_diff>